<commit_message>
work for 8th of August
</commit_message>
<xml_diff>
--- a/空白人物卡.xlsx
+++ b/空白人物卡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitStuff\Tao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AACD92-043A-45D2-B9F4-E8D3F0873491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74999934-C34E-4E39-8614-3203C2536AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,20 +459,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,7 +757,7 @@
   <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -779,12 +779,12 @@
       <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="10">
         <v>0.5</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -917,13 +917,13 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1085,7 +1085,7 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1405,57 +1405,57 @@
       <c r="A48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -1466,97 +1466,97 @@
       <c r="A55" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -1618,13 +1618,13 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
@@ -1671,30 +1671,38 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
       <c r="F80" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B9:G13"/>
     <mergeCell ref="A73:G73"/>
     <mergeCell ref="A79:G79"/>
     <mergeCell ref="B80:E80"/>
@@ -1706,14 +1714,6 @@
     <mergeCell ref="B58:G60"/>
     <mergeCell ref="B61:G63"/>
     <mergeCell ref="A64:G64"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B9:G13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G4">

</xml_diff>